<commit_message>
update imputation mandatory status for curator template
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.11.xlsx
+++ b/schema_definitions/template_schema_v1.11.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhayhurst/Documents/git/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C666B6-DEF1-5247-96A5-3AC9908454A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0940D1-34B7-1342-9CE7-0D8178A484CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11800" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="3" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="-11800" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -802,25 +802,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1138,88 +1137,85 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="80.6640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="22" style="5" customWidth="1"/>
-    <col min="8" max="8" width="28.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="5"/>
-    <col min="10" max="10" width="16.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.83203125" style="5"/>
-    <col min="14" max="14" width="23.6640625" style="5" customWidth="1"/>
-    <col min="15" max="16" width="44.5" style="6" customWidth="1"/>
-    <col min="17" max="17" width="96" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.83203125" style="11"/>
-    <col min="19" max="16384" width="10.83203125" style="5"/>
+    <col min="1" max="1" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.6640625" customWidth="1"/>
+    <col min="15" max="16" width="44.5" style="5" customWidth="1"/>
+    <col min="17" max="17" width="96" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" t="s">
         <v>152</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" t="s">
         <v>177</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" t="s">
         <v>178</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" t="s">
         <v>151</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>167</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="R1" s="10" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1228,83 +1224,83 @@
       <c r="C2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" t="s">
         <v>222</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R2" s="11">
+      <c r="O2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2" s="10">
         <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" t="s">
         <v>142</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" t="s">
         <v>159</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" t="s">
         <v>140</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" t="s">
         <v>141</v>
       </c>
-      <c r="O3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R3" s="11">
+      <c r="O3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R3" s="10">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1313,690 +1309,690 @@
       <c r="C4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="5" t="s">
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
         <v>24</v>
       </c>
       <c r="K4" s="1"/>
-      <c r="N4" s="5" t="s">
+      <c r="N4" t="s">
         <v>31</v>
       </c>
-      <c r="O4" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="P4" s="6" t="s">
+      <c r="O4" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P4" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" t="s">
         <v>189</v>
       </c>
-      <c r="R4" s="11">
+      <c r="R4" s="10">
         <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5" t="s">
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
         <v>24</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" t="s">
         <v>32</v>
       </c>
-      <c r="O5" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="P5" s="9" t="s">
+      <c r="O5" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="P5" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="Q5" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="R5" s="11">
+      <c r="R5" s="10">
         <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5" t="s">
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" t="s">
         <v>222</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="N6" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="P6" s="9"/>
-      <c r="R6" s="11">
+      <c r="O6" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" s="8"/>
+      <c r="R6" s="10">
         <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" t="s">
         <v>202</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C7" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5" t="s">
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" t="s">
         <v>222</v>
       </c>
       <c r="K7" s="1"/>
-      <c r="N7" s="5" t="s">
+      <c r="N7" t="s">
         <v>204</v>
       </c>
-      <c r="O7" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="P7" s="9"/>
-      <c r="R7" s="11">
+      <c r="O7" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="P7" s="8"/>
+      <c r="R7" s="10">
         <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5" t="b">
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="b">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="5" t="s">
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
         <v>43</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8" t="s">
         <v>34</v>
       </c>
-      <c r="O8" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="5" t="s">
+      <c r="O8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="s">
         <v>44</v>
       </c>
-      <c r="R8" s="11">
+      <c r="R8" s="10">
         <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" t="s">
         <v>205</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>206</v>
       </c>
-      <c r="C9" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" s="5" t="b">
-        <v>1</v>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
       </c>
       <c r="G9" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="5" t="s">
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" t="s">
         <v>222</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="N9" s="5" t="s">
+      <c r="N9" t="s">
         <v>206</v>
       </c>
-      <c r="O9" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R9" s="11">
+      <c r="O9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R9" s="10">
         <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" t="s">
         <v>208</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>207</v>
       </c>
-      <c r="C10" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" s="5" t="b">
-        <v>1</v>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
       </c>
       <c r="G10" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5" t="s">
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" t="s">
         <v>222</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="N10" s="5" t="s">
+      <c r="N10" t="s">
         <v>207</v>
       </c>
-      <c r="O10" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R10" s="11">
+      <c r="O10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R10" s="10">
         <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" s="5" t="s">
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
         <v>57</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="N11" t="s">
         <v>35</v>
       </c>
-      <c r="O11" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R11" s="11">
+      <c r="O11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R11" s="10">
         <v>-1</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="5" t="s">
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="J12" t="s">
         <v>222</v>
       </c>
-      <c r="N12" s="5" t="s">
+      <c r="N12" t="s">
         <v>36</v>
       </c>
-      <c r="O12" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R12" s="11">
+      <c r="O12" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R12" s="10">
         <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" s="5" t="s">
+      <c r="C13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
         <v>24</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="J13" t="s">
         <v>222</v>
       </c>
-      <c r="N13" s="5" t="s">
+      <c r="N13" t="s">
         <v>37</v>
       </c>
-      <c r="O13" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R13" s="11">
+      <c r="O13" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R13" s="10">
         <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="A14" t="s">
         <v>218</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" t="s">
         <v>219</v>
       </c>
-      <c r="C14" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" s="5" t="s">
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
         <v>24</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="J14" t="s">
         <v>222</v>
       </c>
-      <c r="N14" s="5" t="s">
+      <c r="N14" t="s">
         <v>220</v>
       </c>
-      <c r="O14" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="P14" s="6" t="s">
+      <c r="O14" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P14" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="R14" s="11">
+      <c r="R14" s="10">
         <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D15" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F15" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I15" s="5" t="s">
+      <c r="C15" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
         <v>24</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="K15" t="s">
         <v>53</v>
       </c>
-      <c r="N15" s="5" t="s">
+      <c r="N15" t="s">
         <v>153</v>
       </c>
-      <c r="O15" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R15" s="11">
+      <c r="O15" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R15" s="10">
         <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" t="s">
         <v>85</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" t="s">
         <v>144</v>
       </c>
-      <c r="C16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="5" t="s">
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
         <v>24</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="J16" t="s">
         <v>222</v>
       </c>
-      <c r="N16" s="5" t="s">
+      <c r="N16" t="s">
         <v>145</v>
       </c>
-      <c r="O16" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="R16" s="11">
+      <c r="O16" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="R16" s="10">
         <v>-1</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="A17" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D17" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F17" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G17" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" s="5" t="s">
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="J17" t="s">
         <v>222</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="K17" t="s">
         <v>54</v>
       </c>
-      <c r="N17" s="5" t="s">
+      <c r="N17" t="s">
         <v>38</v>
       </c>
-      <c r="O17" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="P17" s="6" t="s">
+      <c r="O17" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P17" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="R17" s="11">
+      <c r="R17" s="10">
         <v>255</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E18" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F18" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G18" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" s="5" t="s">
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="J18" t="s">
         <v>222</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="K18" t="s">
         <v>56</v>
       </c>
-      <c r="N18" s="5" t="s">
+      <c r="N18" t="s">
         <v>39</v>
       </c>
-      <c r="O18" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R18" s="11">
+      <c r="O18" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R18" s="10">
         <v>255</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E19" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F19" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G19" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" s="5" t="s">
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
         <v>24</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="J19" t="s">
         <v>222</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="K19" t="s">
         <v>55</v>
       </c>
-      <c r="N19" s="5" t="s">
+      <c r="N19" t="s">
         <v>40</v>
       </c>
-      <c r="O19" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="P19" s="6" t="s">
+      <c r="O19" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P19" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="R19" s="11">
+      <c r="R19" s="10">
         <v>255</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="A20" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2005,341 +2001,341 @@
       <c r="C20" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D20" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E20" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F20" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G20" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I20" s="5" t="s">
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" t="s">
         <v>24</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="J20" t="s">
         <v>221</v>
       </c>
-      <c r="N20" s="5" t="s">
+      <c r="N20" t="s">
         <v>41</v>
       </c>
-      <c r="O20" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R20" s="11">
+      <c r="O20" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R20" s="10">
         <v>255</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="A21" t="s">
         <v>157</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" t="s">
         <v>175</v>
       </c>
-      <c r="C21" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D21" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E21" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F21" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G21" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H21" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" s="5" t="s">
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
         <v>24</v>
       </c>
-      <c r="J21" s="5" t="s">
+      <c r="J21" t="s">
         <v>222</v>
       </c>
-      <c r="N21" s="5" t="s">
+      <c r="N21" t="s">
         <v>61</v>
       </c>
-      <c r="O21" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R21" s="11">
+      <c r="O21" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R21" s="10">
         <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="A22" t="s">
         <v>187</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" t="s">
         <v>186</v>
       </c>
-      <c r="C22" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D22" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E22" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F22" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G22" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H22" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I22" s="5" t="s">
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22" t="b">
+        <v>0</v>
+      </c>
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
         <v>24</v>
       </c>
-      <c r="J22" s="5" t="s">
+      <c r="J22" t="s">
         <v>223</v>
       </c>
-      <c r="N22" s="5" t="s">
+      <c r="N22" t="s">
         <v>188</v>
       </c>
-      <c r="O22" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="R22" s="11">
+      <c r="O22" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="R22" s="10">
         <v>-1</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+      <c r="A23" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" t="s">
         <v>176</v>
       </c>
-      <c r="C23" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E23" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F23" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G23" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I23" s="5" t="s">
+      <c r="C23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" t="b">
+        <v>0</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
         <v>24</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="K23" t="s">
         <v>51</v>
       </c>
-      <c r="N23" s="5" t="s">
+      <c r="N23" t="s">
         <v>52</v>
       </c>
-      <c r="O23" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="5" t="s">
+      <c r="O23" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="s">
         <v>165</v>
       </c>
-      <c r="R23" s="11">
+      <c r="R23" s="10">
         <v>255</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+      <c r="A24" t="s">
         <v>215</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" t="s">
         <v>216</v>
       </c>
-      <c r="C24" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D24" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E24" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F24" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G24" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H24" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I24" s="5" t="s">
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
         <v>43</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="N24" s="5" t="s">
+      <c r="N24" t="s">
         <v>217</v>
       </c>
-      <c r="O24" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="5" t="s">
+      <c r="O24" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="s">
         <v>44</v>
       </c>
-      <c r="R24" s="11">
+      <c r="R24" s="10">
         <v>-1</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
+      <c r="A25" t="s">
         <v>209</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" t="s">
         <v>210</v>
       </c>
-      <c r="C25" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D25" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E25" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F25" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G25" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H25" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I25" s="5" t="s">
+      <c r="C25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" t="s">
         <v>99</v>
       </c>
-      <c r="N25" s="5" t="s">
+      <c r="N25" t="s">
         <v>211</v>
       </c>
-      <c r="O25" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R25" s="11">
+      <c r="O25" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R25" s="10">
         <v>-1</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+      <c r="A26" t="s">
         <v>146</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" t="s">
         <v>169</v>
       </c>
-      <c r="C26" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D26" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E26" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F26" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G26" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H26" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I26" s="5" t="s">
+      <c r="C26" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26" t="b">
+        <v>0</v>
+      </c>
+      <c r="F26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
         <v>24</v>
       </c>
-      <c r="J26" s="5" t="s">
+      <c r="J26" t="s">
         <v>222</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="K26" t="s">
         <v>147</v>
       </c>
-      <c r="N26" s="5" t="s">
+      <c r="N26" t="s">
         <v>154</v>
       </c>
-      <c r="O26" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="P26" s="6" t="s">
+      <c r="O26" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P26" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="R26" s="11">
+      <c r="R26" s="10">
         <v>255</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+      <c r="A27" t="s">
         <v>148</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" t="s">
         <v>170</v>
       </c>
-      <c r="C27" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D27" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E27" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F27" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G27" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H27" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I27" s="5" t="s">
+      <c r="C27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
         <v>24</v>
       </c>
-      <c r="J27" s="5" t="s">
+      <c r="J27" t="s">
         <v>222</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="K27" t="s">
         <v>149</v>
       </c>
-      <c r="N27" s="5" t="s">
+      <c r="N27" t="s">
         <v>150</v>
       </c>
-      <c r="O27" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="P27" s="6" t="s">
+      <c r="O27" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P27" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="R27" s="11">
+      <c r="R27" s="10">
         <v>255</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="A28" t="s">
         <v>183</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2348,166 +2344,166 @@
       <c r="C28" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="D28" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E28" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F28" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G28" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H28" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I28" s="5" t="s">
+      <c r="D28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" t="b">
+        <v>0</v>
+      </c>
+      <c r="F28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" t="b">
+        <v>0</v>
+      </c>
+      <c r="H28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
         <v>24</v>
       </c>
-      <c r="J28" s="5" t="s">
+      <c r="J28" t="s">
         <v>221</v>
       </c>
-      <c r="N28" s="5" t="s">
+      <c r="N28" t="s">
         <v>184</v>
       </c>
-      <c r="O28" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R28" s="11">
+      <c r="O28" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R28" s="10">
         <v>-1</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+      <c r="A29" t="s">
         <v>192</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" t="s">
         <v>193</v>
       </c>
-      <c r="C29" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D29" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E29" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F29" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G29" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H29" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I29" s="5" t="s">
+      <c r="C29" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" t="b">
+        <v>0</v>
+      </c>
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+      <c r="G29" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" t="s">
         <v>43</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="N29" s="5" t="s">
+      <c r="N29" t="s">
         <v>196</v>
       </c>
-      <c r="O29" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="5" t="s">
+      <c r="O29" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q29" t="s">
         <v>44</v>
       </c>
-      <c r="R29" s="11">
+      <c r="R29" s="10">
         <v>-1</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
+      <c r="A30" t="s">
         <v>191</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" t="s">
         <v>194</v>
       </c>
-      <c r="C30" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D30" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F30" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G30" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H30" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I30" s="5" t="s">
+      <c r="C30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
         <v>43</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="N30" s="5" t="s">
+      <c r="N30" t="s">
         <v>197</v>
       </c>
-      <c r="O30" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="5" t="s">
+      <c r="O30" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="s">
         <v>44</v>
       </c>
-      <c r="R30" s="11">
+      <c r="R30" s="10">
         <v>-1</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
+      <c r="A31" t="s">
         <v>190</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" t="s">
         <v>195</v>
       </c>
-      <c r="C31" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D31" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F31" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G31" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H31" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I31" s="5" t="s">
+      <c r="C31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" t="b">
+        <v>0</v>
+      </c>
+      <c r="F31" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" t="s">
         <v>43</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="N31" s="5" t="s">
+      <c r="N31" t="s">
         <v>198</v>
       </c>
-      <c r="O31" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="5" t="s">
+      <c r="O31" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="s">
         <v>44</v>
       </c>
-      <c r="R31" s="11">
+      <c r="R31" s="10">
         <v>-1</v>
       </c>
     </row>
@@ -2528,683 +2524,681 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="22" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" style="5"/>
-    <col min="12" max="12" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" style="5" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="44.5" style="6" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="5"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="44.5" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" t="s">
         <v>152</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" t="s">
         <v>177</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" t="s">
         <v>178</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" t="s">
         <v>151</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="R1" s="10" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" t="s">
         <v>222</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R2" s="5">
+      <c r="O2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2">
         <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" t="s">
         <v>222</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" t="s">
         <v>136</v>
       </c>
-      <c r="O3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R3" s="5">
+      <c r="O3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R3">
         <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" t="s">
         <v>135</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" t="s">
         <v>134</v>
       </c>
-      <c r="C4" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="5" t="s">
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" t="s">
         <v>222</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" t="s">
         <v>133</v>
       </c>
-      <c r="O4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R4" s="5">
+      <c r="O4" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R4">
         <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" t="s">
         <v>131</v>
       </c>
-      <c r="C5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5" t="s">
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" t="s">
         <v>181</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="L5" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="M5" s="13"/>
-      <c r="N5" s="5" t="s">
+      <c r="M5" s="12"/>
+      <c r="N5" t="s">
         <v>130</v>
       </c>
-      <c r="O5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="P5" s="9"/>
-      <c r="R5" s="12">
+      <c r="O5" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" s="8"/>
+      <c r="R5" s="11">
         <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" t="s">
         <v>129</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" t="s">
         <v>128</v>
       </c>
-      <c r="C6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5" t="s">
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" t="s">
         <v>222</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="N6" t="s">
         <v>156</v>
       </c>
-      <c r="O6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="P6" s="9"/>
-      <c r="R6" s="5">
+      <c r="O6" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" s="8"/>
+      <c r="R6">
         <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" t="s">
         <v>126</v>
       </c>
-      <c r="C7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5" t="s">
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" t="s">
         <v>222</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" t="s">
         <v>125</v>
       </c>
-      <c r="O7" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R7" s="5">
+      <c r="O7" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R7">
         <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" t="s">
         <v>124</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" t="s">
         <v>123</v>
       </c>
-      <c r="C8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="5" t="s">
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" t="s">
         <v>172</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8" t="s">
         <v>122</v>
       </c>
-      <c r="O8" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R8" s="5">
+      <c r="O8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R8">
         <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" t="s">
         <v>121</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>120</v>
       </c>
-      <c r="C9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="5" t="s">
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" t="s">
         <v>172</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9" t="s">
         <v>119</v>
       </c>
-      <c r="O9" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R9" s="5">
+      <c r="O9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R9">
         <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" t="s">
         <v>118</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>117</v>
       </c>
-      <c r="C10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5" t="s">
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
         <v>99</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="N10" t="s">
         <v>116</v>
       </c>
-      <c r="O10" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R10" s="12">
+      <c r="O10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R10" s="11">
         <v>-1</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" t="s">
         <v>115</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>114</v>
       </c>
-      <c r="C11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" s="5" t="s">
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
         <v>99</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="N11" t="s">
         <v>113</v>
       </c>
-      <c r="O11" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R11" s="12">
+      <c r="O11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R11" s="11">
         <v>-1</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" t="s">
         <v>106</v>
       </c>
-      <c r="C12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="5" t="s">
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
         <v>99</v>
       </c>
-      <c r="N12" s="5" t="s">
+      <c r="N12" t="s">
         <v>105</v>
       </c>
-      <c r="O12" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="R12" s="12">
+      <c r="O12" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="R12" s="11">
         <v>-1</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="A13" t="s">
         <v>104</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>103</v>
       </c>
-      <c r="C13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" s="5" t="s">
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
         <v>99</v>
       </c>
-      <c r="N13" s="5" t="s">
+      <c r="N13" t="s">
         <v>102</v>
       </c>
-      <c r="O13" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R13" s="12">
+      <c r="O13" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R13" s="11">
         <v>-1</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="A14" t="s">
         <v>112</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" t="s">
         <v>111</v>
       </c>
-      <c r="C14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" s="5" t="s">
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
         <v>99</v>
       </c>
-      <c r="N14" s="5" t="s">
+      <c r="N14" t="s">
         <v>110</v>
       </c>
-      <c r="O14" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R14" s="12">
+      <c r="O14" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R14" s="11">
         <v>-1</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="A15" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>108</v>
       </c>
-      <c r="C15" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="5" t="s">
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="J15" t="s">
         <v>222</v>
       </c>
-      <c r="N15" s="5" t="s">
+      <c r="N15" t="s">
         <v>108</v>
       </c>
-      <c r="O15" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R15" s="5">
+      <c r="O15" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R15">
         <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" t="s">
         <v>101</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" t="s">
         <v>100</v>
       </c>
-      <c r="C16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="5" t="s">
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
         <v>99</v>
       </c>
-      <c r="N16" s="5" t="s">
+      <c r="N16" t="s">
         <v>98</v>
       </c>
-      <c r="O16" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R16" s="12">
+      <c r="O16" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R16" s="11">
         <v>-1</v>
       </c>
     </row>
     <row r="18" spans="15:15" x14ac:dyDescent="0.2">
-      <c r="O18" s="9"/>
+      <c r="O18" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="C1:C16" xr:uid="{692A23DE-1971-9644-BCB5-0858E868D84D}"/>
@@ -3217,590 +3211,590 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EEE6B5-99CE-7744-8022-5400F74ED3C6}">
   <dimension ref="A1:R1002"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22" style="6" customWidth="1"/>
-    <col min="2" max="2" width="88.1640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="21.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.5" style="6" customWidth="1"/>
-    <col min="11" max="11" width="35.83203125" style="6" customWidth="1"/>
-    <col min="12" max="13" width="10.5" style="6" customWidth="1"/>
-    <col min="14" max="14" width="44.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="44.5" style="6" customWidth="1"/>
-    <col min="17" max="17" width="18.5" style="6" customWidth="1"/>
-    <col min="18" max="32" width="10.5" style="6" customWidth="1"/>
-    <col min="33" max="16384" width="11.1640625" style="6"/>
+    <col min="1" max="1" width="22" style="5" customWidth="1"/>
+    <col min="2" max="2" width="88.1640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="21.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.5" style="5" customWidth="1"/>
+    <col min="11" max="11" width="35.83203125" style="5" customWidth="1"/>
+    <col min="12" max="13" width="10.5" style="5" customWidth="1"/>
+    <col min="14" max="14" width="44.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="44.5" style="5" customWidth="1"/>
+    <col min="17" max="17" width="18.5" style="5" customWidth="1"/>
+    <col min="18" max="32" width="10.5" style="5" customWidth="1"/>
+    <col min="33" max="16384" width="11.1640625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="5" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="C2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" t="s">
         <v>222</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R2" s="6">
+      <c r="O2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2" s="5">
         <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C3" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="6" t="s">
+      <c r="C3" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="O3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="6" t="s">
+      <c r="O3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="R3" s="6">
+      <c r="R3" s="5">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="C4" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="N4" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="O4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R4" s="12">
+      <c r="O4" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R4" s="11">
         <v>-1</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C5" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="9" t="s">
+      <c r="C5" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>43</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="N5" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="O5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="5" t="s">
+      <c r="O5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
         <v>44</v>
       </c>
-      <c r="R5" s="11">
+      <c r="R5" s="10">
         <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="9" t="s">
+      <c r="C6" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="N6" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="O6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="P6" s="9"/>
-      <c r="R6" s="12">
+      <c r="O6" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" s="8"/>
+      <c r="R6" s="11">
         <v>-1</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C7" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="9" t="s">
+      <c r="C7" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="N7" s="9" t="s">
+      <c r="N7" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="O7" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="P7" s="9"/>
-      <c r="R7" s="12">
+      <c r="O7" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="P7" s="8"/>
+      <c r="R7" s="11">
         <v>-1</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="6" t="s">
+      <c r="C8" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" t="s">
         <v>222</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="N8" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="O8" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R8" s="6">
+      <c r="O8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R8" s="5">
         <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="C9" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="6" t="s">
+      <c r="C9" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="K9" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="N9" s="6" t="s">
+      <c r="N9" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="O9" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="P9" s="6" t="s">
+      <c r="O9" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P9" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="Q9" s="6" t="s">
+      <c r="Q9" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="R9" s="6">
+      <c r="R9" s="5">
         <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="6" t="s">
+      <c r="C10" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" t="s">
         <v>222</v>
       </c>
-      <c r="N10" s="6" t="s">
+      <c r="N10" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O10" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R10" s="6">
+      <c r="O10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R10" s="5">
         <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" s="6" t="s">
+      <c r="C11" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" t="s">
         <v>222</v>
       </c>
-      <c r="N11" s="6" t="s">
+      <c r="N11" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="O11" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R11" s="6">
+      <c r="O11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R11" s="5">
         <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C12" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="6" t="s">
+      <c r="C12" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="J12" t="s">
         <v>222</v>
       </c>
-      <c r="N12" s="6" t="s">
+      <c r="N12" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="O12" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="P12" s="6" t="s">
+      <c r="O12" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P12" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="R12" s="6">
+      <c r="R12" s="5">
         <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" s="6" t="s">
+      <c r="C13" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="6" t="s">
+      <c r="K13" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="N13" s="6" t="s">
+      <c r="N13" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="O13" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="P13" s="6" t="s">
+      <c r="O13" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P13" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="Q13" s="6" t="s">
+      <c r="Q13" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="R13" s="6">
+      <c r="R13" s="5">
         <v>255</v>
       </c>
     </row>
@@ -4803,86 +4797,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED4CB50-F135-6F43-A6BC-AC27D4D7EACE}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+    <sheetView zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.1640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="22.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="5"/>
-    <col min="10" max="10" width="16.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.83203125" style="5"/>
-    <col min="14" max="14" width="23.6640625" style="5" customWidth="1"/>
-    <col min="15" max="16" width="44.5" style="6" customWidth="1"/>
-    <col min="17" max="17" width="140.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="5"/>
+    <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.1640625" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.6640625" customWidth="1"/>
+    <col min="15" max="16" width="44.5" style="5" customWidth="1"/>
+    <col min="17" max="17" width="140.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" t="s">
         <v>152</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" t="s">
         <v>177</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" t="s">
         <v>178</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" t="s">
         <v>151</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>167</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="5" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -4891,173 +4882,173 @@
       <c r="C2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="D2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" t="s">
         <v>222</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R2" s="5">
+      <c r="O2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2">
         <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" t="s">
         <v>69</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="D3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="D3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" t="s">
         <v>223</v>
       </c>
       <c r="K3" s="1"/>
-      <c r="N3" s="5" t="s">
+      <c r="N3" t="s">
         <v>68</v>
       </c>
-      <c r="O3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R3" s="5">
+      <c r="O3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R3">
         <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" t="s">
         <v>67</v>
       </c>
       <c r="C4" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="D4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="5" t="s">
+      <c r="D4" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
         <v>24</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" t="s">
         <v>66</v>
       </c>
-      <c r="O4" s="6" t="b">
+      <c r="O4" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="R4" s="5">
+      <c r="R4">
         <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" t="s">
         <v>64</v>
       </c>
       <c r="C5" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="D5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5" t="s">
+      <c r="D5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
         <v>24</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" t="s">
         <v>63</v>
       </c>
-      <c r="O5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="P5" s="9"/>
+      <c r="O5" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" s="8"/>
       <c r="Q5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="R5" s="5">
+      <c r="R5">
         <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="6"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="5"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>

</xml_diff>

<commit_message>
add genotyping tech to sumstats study sheet
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.11.xlsx
+++ b/schema_definitions/template_schema_v1.11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhayhurst/Documents/git/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0940D1-34B7-1342-9CE7-0D8178A484CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2DACD1-E100-4046-9EDF-E2CEF74FC933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-11800" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
@@ -1137,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="241" zoomScaleNormal="241" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1322,7 +1322,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" t="s">
         <v>24</v>
@@ -3211,8 +3211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EEE6B5-99CE-7744-8022-5400F74ED3C6}">
   <dimension ref="A1:R1002"/>
   <sheetViews>
-    <sheetView zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>